<commit_message>
Met à jour attributions.xslx
</commit_message>
<xml_diff>
--- a/src/main/uml/attributions.xlsx
+++ b/src/main/uml/attributions.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Formateur\Documents\NetBeansProjects\SIOMassy2022\src\main\uml\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Le formateur crée un exercice à faire en groupe (EFG). [2]</t>
   </si>
@@ -165,13 +160,16 @@
   </si>
   <si>
     <t>L'étudiant répond à un questionnaire. [2], à fusionner avec « liste ses »</t>
+  </si>
+  <si>
+    <t>Tamby</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,7 +263,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -300,7 +298,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -477,32 +475,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="77.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -510,7 +508,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="30">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -518,7 +516,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -526,7 +524,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -534,7 +532,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -542,7 +540,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -550,7 +548,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -558,7 +556,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -566,7 +564,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -574,7 +572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -582,22 +580,28 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="30">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -605,7 +609,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
@@ -613,17 +617,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -631,7 +635,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -639,12 +643,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -652,12 +656,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -665,7 +669,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
@@ -673,7 +677,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
         <v>39</v>
       </c>
@@ -681,7 +685,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="30">
       <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
@@ -689,12 +693,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
@@ -702,7 +706,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="30">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
@@ -710,12 +714,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -723,22 +727,22 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" ht="17.25" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Met à jour attributions.xlsx
</commit_message>
<xml_diff>
--- a/src/main/uml/attributions.xlsx
+++ b/src/main/uml/attributions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Le formateur crée un exercice à faire en groupe (EFG). [2]</t>
   </si>
@@ -83,21 +83,12 @@
     <t>Adem</t>
   </si>
   <si>
-    <t>Le formateur pose une question (oui/non, à choix multiples, à saisie libre) [2]</t>
-  </si>
-  <si>
     <t>Cheick</t>
   </si>
   <si>
     <t>Le participant répond à une question [1]</t>
   </si>
   <si>
-    <t>Le participant affiche les réponses à une question [1]</t>
-  </si>
-  <si>
-    <t>Le participant liste les questions du canal [1]</t>
-  </si>
-  <si>
     <t>Dieynaba</t>
   </si>
   <si>
@@ -116,15 +107,9 @@
     <t>David</t>
   </si>
   <si>
-    <t>Le formateur liste ses questionnaires (toutes sessions confondues). [1]</t>
-  </si>
-  <si>
     <t>Nadjia</t>
   </si>
   <si>
-    <t>Le formateur affiche, crée, modifie, supprime un questionnaire. [2]</t>
-  </si>
-  <si>
     <t>Le formateur liste les passages de questionnaire. [2]</t>
   </si>
   <si>
@@ -146,25 +131,43 @@
     <t>Le formateur saisit les notes d'une évaluation. [2]</t>
   </si>
   <si>
-    <t xml:space="preserve">Le membre peut lister les sessions en cours (et en option les anciennes, pour se rappeler d'anciens étudiants). [1] </t>
-  </si>
-  <si>
     <t>Abdillahi</t>
   </si>
   <si>
     <t>L'étudiant s'inscrit sur l'application (confirmation par email). [3]</t>
   </si>
   <si>
-    <t xml:space="preserve">Le gestionnaire ou le formateur l'accepte dans une session de formation (ou l'en retire, si erreur). [2] </t>
-  </si>
-  <si>
     <t>L'administrateur gère les membres d'un canal. [2]</t>
   </si>
   <si>
     <t>Karim</t>
   </si>
   <si>
-    <t>L'étudiant répond à un questionnaire. [2], à fusionner avec « liste ses »</t>
+    <t xml:space="preserve">Le membre peut lister les canaux. [1] </t>
+  </si>
+  <si>
+    <t>Ilyesse</t>
+  </si>
+  <si>
+    <t>Le formateur liste ses questionnaires (tous canaux confondus). [1]</t>
+  </si>
+  <si>
+    <t>Le formateur crée un questionnaire. [2]</t>
+  </si>
+  <si>
+    <t>Le formateur lance un sondage (oui/non, à choix multiples, à saisie libre) [2]</t>
+  </si>
+  <si>
+    <t>Le participant affiche les réponses à un sondage [1]</t>
+  </si>
+  <si>
+    <t>Le participant liste les sondages du canal [1]</t>
+  </si>
+  <si>
+    <t>L'étudiant répond à un questionnaire. [1]</t>
+  </si>
+  <si>
+    <t>Le gestionnaire ou le formateur liste les membres d'un canal [1]</t>
   </si>
 </sst>
 </file>
@@ -488,12 +491,12 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="77.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="78.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -515,7 +518,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -526,17 +529,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -544,42 +547,42 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -591,6 +594,9 @@
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -599,18 +605,15 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -622,21 +625,24 @@
       <c r="A18" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -646,10 +652,10 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -659,34 +665,34 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -696,31 +702,34 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Change une attribution de fonctionnalité
</commit_message>
<xml_diff>
--- a/src/main/uml/attributions.xlsx
+++ b/src/main/uml/attributions.xlsx
@@ -490,9 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -602,6 +600,9 @@
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -640,9 +641,6 @@
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B20" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>